<commit_message>
page history partly done
</commit_message>
<xml_diff>
--- a/test/resources/unittest_DAZHO_1_74.xlsx
+++ b/test/resources/unittest_DAZHO_1_74.xlsx
@@ -924,7 +924,7 @@
     <row r="2" ht="19" customHeight="1">
       <c r="A2" s="42" t="inlineStr">
         <is>
-          <t>Метричні книги Ковельського, Заславського, Дубенського, Ровенського, Овруцького, Кременецького повітів. Сповідальні відомості по Ковельському, Заславському, Дубенському, Ровенському, Овруцькому, Кременецькому повітах</t>
+          <t>Metric books of Kovel, Zaslav, Dubensky, Rivne, Ovruch, Kremenetsky counties. Confessional information on Kovel, Zaslavsky, Dubensky, Rivne, Ovruch, Kremenetsky counties</t>
         </is>
       </c>
       <c r="B2" s="33" t="n"/>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="B8" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги Кашогродського уніатського деканату Ковельського і Луцького повітів</t>
+          <t>Metric books of the Kashogrod Uniate Deanery of Kovel and Lutsk counties</t>
         </is>
       </c>
       <c r="C8" s="49" t="inlineStr">
@@ -1258,7 +1258,7 @@
       </c>
       <c r="B9" s="48" t="inlineStr">
         <is>
-          <t>Сповідні розписи Ратинського уніатського деканату Ковельського повіту</t>
+          <t>Confessional paintings of the Ratin Uniate Deanery of Kovel County</t>
         </is>
       </c>
       <c r="C9" s="49" t="inlineStr">
@@ -1305,7 +1305,7 @@
       </c>
       <c r="B10" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги уніатських церков Ковельського повіту</t>
+          <t>Metric books of the Uniate Churches of Kovel County</t>
         </is>
       </c>
       <c r="C10" s="49" t="inlineStr">
@@ -1352,7 +1352,7 @@
       </c>
       <c r="B11" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги Кашогродського уніатського деканату Ковельського і Луцького повітів</t>
+          <t>Metric books of the Kashogrod Uniate Deanery of Kovel and Lutsk counties</t>
         </is>
       </c>
       <c r="C11" s="49" t="inlineStr">
@@ -1399,7 +1399,7 @@
       </c>
       <c r="B12" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги уніатських церков Ковельського та Луцького повітів</t>
+          <t>Metric books of the Uniate Churches of Kovel and Lutsk counties</t>
         </is>
       </c>
       <c r="C12" s="49" t="inlineStr">
@@ -1446,7 +1446,7 @@
       </c>
       <c r="B13" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга греко-католицької церкви с. Мирин Ковельського повіту</t>
+          <t>Metric book of the Greek Catholic Church. Myrin Kovel County</t>
         </is>
       </c>
       <c r="C13" s="49" t="inlineStr">
@@ -1493,7 +1493,7 @@
       </c>
       <c r="B14" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга греко-католицьких Михайло-Архангельської церкви с. Секунь та Успенської с. Городище Ковельського повіту</t>
+          <t>Metric Book of Greek Catholic Michael-Archangel Church. Sekun and Assumption village. The settlement of Kovel county</t>
         </is>
       </c>
       <c r="C14" s="49" t="inlineStr">
@@ -1540,7 +1540,7 @@
       </c>
       <c r="B15" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги уніатських церков Ковельського повіту</t>
+          <t>Metric books of the Uniate Churches of Kovel County</t>
         </is>
       </c>
       <c r="C15" s="49" t="inlineStr">
@@ -1587,7 +1587,7 @@
       </c>
       <c r="B16" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги уніатських церков Ковельського повіту</t>
+          <t>Metric books of the Uniate Churches of Kovel County</t>
         </is>
       </c>
       <c r="C16" s="49" t="inlineStr">
@@ -1634,7 +1634,7 @@
       </c>
       <c r="B17" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги уніатських церков Ковельського повіту</t>
+          <t>Metric books of the Uniate Churches of Kovel County</t>
         </is>
       </c>
       <c r="C17" s="49" t="inlineStr">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="B18" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги уніатських церков Ковельського повіту</t>
+          <t>Metric books of the Uniate Churches of Kovel County</t>
         </is>
       </c>
       <c r="C18" s="49" t="inlineStr">
@@ -1728,7 +1728,7 @@
       </c>
       <c r="B19" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга про народження, шлюб та смерть</t>
+          <t>Metric Book of Birth, Marriage and Death</t>
         </is>
       </c>
       <c r="C19" s="49" t="inlineStr">
@@ -1775,7 +1775,7 @@
       </c>
       <c r="B20" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги уніатських церков Ковельського повіту</t>
+          <t>Metric books of the Uniate Churches of Kovel County</t>
         </is>
       </c>
       <c r="C20" s="49" t="inlineStr">
@@ -1822,7 +1822,7 @@
       </c>
       <c r="B21" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги уніатських церков Ковельського повіту</t>
+          <t>Metric books of the Uniate Churches of Kovel County</t>
         </is>
       </c>
       <c r="C21" s="49" t="inlineStr">
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B22" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга про народження, шлюб та смерть</t>
+          <t>Metric Book of Birth, Marriage and Death</t>
         </is>
       </c>
       <c r="C22" s="49" t="inlineStr">
@@ -1916,7 +1916,7 @@
       </c>
       <c r="B23" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга про народження, шлюб та смерть</t>
+          <t>Metric Book of Birth, Marriage and Death</t>
         </is>
       </c>
       <c r="C23" s="49" t="inlineStr">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="B24" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга про народження, шлюб та смерть</t>
+          <t>Metric Book of Birth, Marriage and Death</t>
         </is>
       </c>
       <c r="C24" s="49" t="inlineStr">
@@ -2010,7 +2010,7 @@
       </c>
       <c r="B25" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги уніатських церков Ковельського повіту</t>
+          <t>Metric books of the Uniate Churches of Kovel County</t>
         </is>
       </c>
       <c r="C25" s="49" t="inlineStr">
@@ -2057,7 +2057,7 @@
       </c>
       <c r="B26" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги уніатських церков Ковельського повіту</t>
+          <t>Metric books of the Uniate Churches of Kovel County</t>
         </is>
       </c>
       <c r="C26" s="49" t="inlineStr">
@@ -2104,7 +2104,7 @@
       </c>
       <c r="B27" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга про народження, шлюб та смерть</t>
+          <t>Metric Book of Birth, Marriage and Death</t>
         </is>
       </c>
       <c r="C27" s="49" t="inlineStr">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="B28" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга про народження, шлюб та смерть</t>
+          <t>Metric Book of Birth, Marriage and Death</t>
         </is>
       </c>
       <c r="C28" s="49" t="inlineStr">
@@ -2198,7 +2198,7 @@
       </c>
       <c r="B29" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга про народження, шлюб та смерть</t>
+          <t>Metric Book of Birth, Marriage and Death</t>
         </is>
       </c>
       <c r="C29" s="49" t="inlineStr">
@@ -2245,7 +2245,7 @@
       </c>
       <c r="B30" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги уніатських церков Ковельського повіту</t>
+          <t>Metric books of the Uniate Churches of Kovel County</t>
         </is>
       </c>
       <c r="C30" s="49" t="inlineStr">
@@ -2292,7 +2292,7 @@
       </c>
       <c r="B31" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга про народження, шлюб та смерть</t>
+          <t>Metric Book of Birth, Marriage and Death</t>
         </is>
       </c>
       <c r="C31" s="49" t="inlineStr">
@@ -2339,7 +2339,7 @@
       </c>
       <c r="B32" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга про народження, шлюб та смерть</t>
+          <t>Metric Book of Birth, Marriage and Death</t>
         </is>
       </c>
       <c r="C32" s="49" t="inlineStr">
@@ -2386,7 +2386,7 @@
       </c>
       <c r="B33" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги уніатських церков Ковельського повіту</t>
+          <t>Metric books of the Uniate Churches of Kovel County</t>
         </is>
       </c>
       <c r="C33" s="49" t="inlineStr">
@@ -2433,7 +2433,7 @@
       </c>
       <c r="B34" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Ковельського повіту</t>
+          <t>Metric books of Orthodox churches of Kovel county</t>
         </is>
       </c>
       <c r="C34" s="49" t="inlineStr">
@@ -2480,7 +2480,7 @@
       </c>
       <c r="B35" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга про народження, шлюб та смерть</t>
+          <t>Metric Book of Birth, Marriage and Death</t>
         </is>
       </c>
       <c r="C35" s="49" t="inlineStr">
@@ -2527,7 +2527,7 @@
       </c>
       <c r="B36" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Ковельського повіту</t>
+          <t>Metric books of Orthodox churches of Kovel county</t>
         </is>
       </c>
       <c r="C36" s="49" t="inlineStr">
@@ -2574,7 +2574,7 @@
       </c>
       <c r="B37" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні розписи православних церков. Села К–Н</t>
+          <t>Confessional paintings of Orthodox churches. The villages of K -N</t>
         </is>
       </c>
       <c r="C37" s="49" t="inlineStr">
@@ -2621,7 +2621,7 @@
       </c>
       <c r="B38" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні розписи православних церков. Села О–Я</t>
+          <t>Confessional paintings of Orthodox churches. The villages of O -I</t>
         </is>
       </c>
       <c r="C38" s="49" t="inlineStr">
@@ -2668,7 +2668,7 @@
       </c>
       <c r="B39" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні розписи православних церков. Села Б–Ж</t>
+          <t>Confessional paintings of Orthodox churches. Village B -D</t>
         </is>
       </c>
       <c r="C39" s="49" t="inlineStr">
@@ -2715,7 +2715,7 @@
       </c>
       <c r="B40" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні розписи православних церков. Села Ж–М</t>
+          <t>Confessional paintings of Orthodox churches. The village of Zh -M</t>
         </is>
       </c>
       <c r="C40" s="49" t="inlineStr">
@@ -2762,7 +2762,7 @@
       </c>
       <c r="B41" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні розписи православних церков Ковельського повіту. Села Ж–Л</t>
+          <t>Confessional paintings of the Orthodox churches of Kovel county. The village of Zh -l</t>
         </is>
       </c>
       <c r="C41" s="49" t="inlineStr">
@@ -2809,7 +2809,7 @@
       </c>
       <c r="B42" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні розписи православних церков Ковельського повіту. Села М–Р</t>
+          <t>Confessional paintings of the Orthodox churches of Kovel county. The villages of the m -p</t>
         </is>
       </c>
       <c r="C42" s="49" t="inlineStr">
@@ -2856,7 +2856,7 @@
       </c>
       <c r="B43" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні розписи православних церков. Села Р–Я</t>
+          <t>Confessional paintings of Orthodox churches. The villages of the r -Y</t>
         </is>
       </c>
       <c r="C43" s="49" t="inlineStr">
@@ -2903,7 +2903,7 @@
       </c>
       <c r="B44" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга Св. Дмитровської греко-католицької церкви по м. Судилків</t>
+          <t>Metric Book of St. Dmitry Greek Catholic Church in Sudylkov</t>
         </is>
       </c>
       <c r="C44" s="49" t="inlineStr">
@@ -2950,7 +2950,7 @@
       </c>
       <c r="B45" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга Св. Троїцької греко-католицької церкви по м. Сульжин</t>
+          <t>Metric Book of St. Trinity Greek Catholic Church in Sulzhin</t>
         </is>
       </c>
       <c r="C45" s="49" t="inlineStr">
@@ -2997,7 +2997,7 @@
       </c>
       <c r="B46" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга грекокатолицької церкви Різдва Пресвятої Богородиці с. Великі Мацевичі</t>
+          <t>Metric Book of the Greek Catholic Church of the Nativity of the Blessed Virgin Mary Great Matsevichi</t>
         </is>
       </c>
       <c r="C46" s="49" t="inlineStr">
@@ -3044,7 +3044,7 @@
       </c>
       <c r="B47" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні по с. Великі Топори</t>
+          <t>Metric books Orthodox on the village. Large toporas</t>
         </is>
       </c>
       <c r="C47" s="49" t="inlineStr">
@@ -3091,7 +3091,7 @@
       </c>
       <c r="B48" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C48" s="49" t="inlineStr">
@@ -3138,7 +3138,7 @@
       </c>
       <c r="B49" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Запславського та Острозького повітів</t>
+          <t>Metric books of Orthodox churches of Zdslav and Ostroh counties</t>
         </is>
       </c>
       <c r="C49" s="49" t="inlineStr">
@@ -3185,7 +3185,7 @@
       </c>
       <c r="B50" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C50" s="49" t="inlineStr">
@@ -3232,7 +3232,7 @@
       </c>
       <c r="B51" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C51" s="49" t="inlineStr">
@@ -3279,7 +3279,7 @@
       </c>
       <c r="B52" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C52" s="49" t="inlineStr">
@@ -3311,7 +3311,7 @@
       </c>
       <c r="B53" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C53" s="49" t="inlineStr">
@@ -3343,7 +3343,7 @@
       </c>
       <c r="B54" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C54" s="49" t="inlineStr">
@@ -3375,7 +3375,7 @@
       </c>
       <c r="B55" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C55" s="49" t="inlineStr">
@@ -3407,7 +3407,7 @@
       </c>
       <c r="B56" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C56" s="49" t="inlineStr">
@@ -3439,7 +3439,7 @@
       </c>
       <c r="B57" s="48" t="inlineStr">
         <is>
-          <t>Шлюбні обшуки православні с. Топори</t>
+          <t>Marriage searches Orthodox. Toporas</t>
         </is>
       </c>
       <c r="C57" s="49" t="inlineStr">
@@ -3471,7 +3471,7 @@
       </c>
       <c r="B58" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C58" s="49" t="inlineStr">
@@ -3503,7 +3503,7 @@
       </c>
       <c r="B59" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C59" s="49" t="inlineStr">
@@ -3535,7 +3535,7 @@
       </c>
       <c r="B60" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C60" s="49" t="inlineStr">
@@ -3567,7 +3567,7 @@
       </c>
       <c r="B61" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C61" s="49" t="inlineStr">
@@ -3599,7 +3599,7 @@
       </c>
       <c r="B62" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C62" s="49" t="inlineStr">
@@ -3631,7 +3631,7 @@
       </c>
       <c r="B63" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C63" s="49" t="inlineStr">
@@ -3663,7 +3663,7 @@
       </c>
       <c r="B64" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C64" s="49" t="inlineStr">
@@ -3695,7 +3695,7 @@
       </c>
       <c r="B65" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C65" s="49" t="inlineStr">
@@ -3727,7 +3727,7 @@
       </c>
       <c r="B66" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C66" s="49" t="inlineStr">
@@ -3759,7 +3759,7 @@
       </c>
       <c r="B67" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C67" s="49" t="inlineStr">
@@ -3791,7 +3791,7 @@
       </c>
       <c r="B68" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C68" s="49" t="inlineStr">
@@ -3823,7 +3823,7 @@
       </c>
       <c r="B69" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C69" s="49" t="inlineStr">
@@ -3855,7 +3855,7 @@
       </c>
       <c r="B70" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C70" s="49" t="inlineStr">
@@ -3887,7 +3887,7 @@
       </c>
       <c r="B71" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C71" s="49" t="inlineStr">
@@ -3919,7 +3919,7 @@
       </c>
       <c r="B72" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C72" s="49" t="inlineStr">
@@ -3951,7 +3951,7 @@
       </c>
       <c r="B73" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C73" s="49" t="inlineStr">
@@ -3983,7 +3983,7 @@
       </c>
       <c r="B74" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C74" s="49" t="inlineStr">
@@ -4015,7 +4015,7 @@
       </c>
       <c r="B75" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C75" s="49" t="inlineStr">
@@ -4047,7 +4047,7 @@
       </c>
       <c r="B76" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C76" s="49" t="inlineStr">
@@ -4079,7 +4079,7 @@
       </c>
       <c r="B77" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C77" s="49" t="inlineStr">
@@ -4111,7 +4111,7 @@
       </c>
       <c r="B78" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C78" s="49" t="inlineStr">
@@ -4143,7 +4143,7 @@
       </c>
       <c r="B79" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C79" s="49" t="inlineStr">
@@ -4175,7 +4175,7 @@
       </c>
       <c r="B80" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C80" s="49" t="inlineStr">
@@ -4207,7 +4207,7 @@
       </c>
       <c r="B81" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C81" s="49" t="inlineStr">
@@ -4239,7 +4239,7 @@
       </c>
       <c r="B82" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C82" s="49" t="inlineStr">
@@ -4271,7 +4271,7 @@
       </c>
       <c r="B83" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C83" s="49" t="inlineStr">
@@ -4303,7 +4303,7 @@
       </c>
       <c r="B84" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C84" s="49" t="inlineStr">
@@ -4335,7 +4335,7 @@
       </c>
       <c r="B85" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C85" s="49" t="inlineStr">
@@ -4367,7 +4367,7 @@
       </c>
       <c r="B86" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C86" s="49" t="inlineStr">
@@ -4399,7 +4399,7 @@
       </c>
       <c r="B87" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C87" s="49" t="inlineStr">
@@ -4431,7 +4431,7 @@
       </c>
       <c r="B88" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C88" s="49" t="inlineStr">
@@ -4463,7 +4463,7 @@
       </c>
       <c r="B89" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C89" s="49" t="inlineStr">
@@ -4495,7 +4495,7 @@
       </c>
       <c r="B90" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C90" s="49" t="inlineStr">
@@ -4527,7 +4527,7 @@
       </c>
       <c r="B91" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C91" s="49" t="inlineStr">
@@ -4559,7 +4559,7 @@
       </c>
       <c r="B92" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C92" s="49" t="inlineStr">
@@ -4591,7 +4591,7 @@
       </c>
       <c r="B93" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C93" s="49" t="inlineStr">
@@ -4623,7 +4623,7 @@
       </c>
       <c r="B94" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C94" s="49" t="inlineStr">
@@ -4655,7 +4655,7 @@
       </c>
       <c r="B95" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C95" s="49" t="inlineStr">
@@ -4687,7 +4687,7 @@
       </c>
       <c r="B96" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C96" s="49" t="inlineStr">
@@ -4719,7 +4719,7 @@
       </c>
       <c r="B97" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C97" s="49" t="inlineStr">
@@ -4746,12 +4746,12 @@
     <row r="98">
       <c r="A98" s="47" t="inlineStr">
         <is>
-          <t>90а</t>
+          <t>90a</t>
         </is>
       </c>
       <c r="B98" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C98" s="49" t="inlineStr">
@@ -4783,7 +4783,7 @@
       </c>
       <c r="B99" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C99" s="49" t="inlineStr">
@@ -4815,7 +4815,7 @@
       </c>
       <c r="B100" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C100" s="49" t="inlineStr">
@@ -4847,7 +4847,7 @@
       </c>
       <c r="B101" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C101" s="49" t="inlineStr">
@@ -4879,7 +4879,7 @@
       </c>
       <c r="B102" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C102" s="49" t="inlineStr">
@@ -4911,7 +4911,7 @@
       </c>
       <c r="B103" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C103" s="49" t="inlineStr">
@@ -4943,7 +4943,7 @@
       </c>
       <c r="B104" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C104" s="49" t="inlineStr">
@@ -4975,7 +4975,7 @@
       </c>
       <c r="B105" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C105" s="49" t="inlineStr">
@@ -5007,7 +5007,7 @@
       </c>
       <c r="B106" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C106" s="49" t="inlineStr">
@@ -5039,7 +5039,7 @@
       </c>
       <c r="B107" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C107" s="49" t="inlineStr">
@@ -5071,7 +5071,7 @@
       </c>
       <c r="B108" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C108" s="49" t="inlineStr">
@@ -5103,7 +5103,7 @@
       </c>
       <c r="B109" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C109" s="49" t="inlineStr">
@@ -5135,7 +5135,7 @@
       </c>
       <c r="B110" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C110" s="49" t="inlineStr">
@@ -5167,7 +5167,7 @@
       </c>
       <c r="B111" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C111" s="49" t="inlineStr">
@@ -5199,7 +5199,7 @@
       </c>
       <c r="B112" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C112" s="49" t="inlineStr">
@@ -5226,12 +5226,12 @@
     <row r="113">
       <c r="A113" s="47" t="inlineStr">
         <is>
-          <t>104а</t>
+          <t>104a</t>
         </is>
       </c>
       <c r="B113" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C113" s="49" t="inlineStr">
@@ -5263,7 +5263,7 @@
       </c>
       <c r="B114" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C114" s="49" t="inlineStr">
@@ -5295,7 +5295,7 @@
       </c>
       <c r="B115" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C115" s="49" t="inlineStr">
@@ -5327,7 +5327,7 @@
       </c>
       <c r="B116" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C116" s="49" t="inlineStr">
@@ -5359,7 +5359,7 @@
       </c>
       <c r="B117" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C117" s="49" t="inlineStr">
@@ -5391,7 +5391,7 @@
       </c>
       <c r="B118" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C118" s="49" t="inlineStr">
@@ -5423,7 +5423,7 @@
       </c>
       <c r="B119" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C119" s="49" t="inlineStr">
@@ -5455,7 +5455,7 @@
       </c>
       <c r="B120" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C120" s="49" t="inlineStr">
@@ -5487,7 +5487,7 @@
       </c>
       <c r="B121" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C121" s="49" t="inlineStr">
@@ -5519,7 +5519,7 @@
       </c>
       <c r="B122" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C122" s="49" t="inlineStr">
@@ -5551,7 +5551,7 @@
       </c>
       <c r="B123" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту</t>
+          <t>Metric books of Orthodox Churches of Zaslavsky County</t>
         </is>
       </c>
       <c r="C123" s="49" t="inlineStr">
@@ -5583,7 +5583,7 @@
       </c>
       <c r="B124" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C124" s="49" t="inlineStr">
@@ -5615,7 +5615,7 @@
       </c>
       <c r="B125" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C125" s="49" t="inlineStr">
@@ -5647,7 +5647,7 @@
       </c>
       <c r="B126" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C126" s="49" t="inlineStr">
@@ -5679,7 +5679,7 @@
       </c>
       <c r="B127" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C127" s="49" t="inlineStr">
@@ -5711,7 +5711,7 @@
       </c>
       <c r="B128" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C128" s="49" t="inlineStr">
@@ -5743,7 +5743,7 @@
       </c>
       <c r="B129" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C129" s="49" t="inlineStr">
@@ -5775,7 +5775,7 @@
       </c>
       <c r="B130" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C130" s="49" t="inlineStr">
@@ -5807,7 +5807,7 @@
       </c>
       <c r="B131" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C131" s="49" t="inlineStr">
@@ -5839,7 +5839,7 @@
       </c>
       <c r="B132" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C132" s="49" t="inlineStr">
@@ -5871,7 +5871,7 @@
       </c>
       <c r="B133" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C133" s="49" t="inlineStr">
@@ -5903,7 +5903,7 @@
       </c>
       <c r="B134" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C134" s="49" t="inlineStr">
@@ -5935,7 +5935,7 @@
       </c>
       <c r="B135" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C135" s="49" t="inlineStr">
@@ -5967,7 +5967,7 @@
       </c>
       <c r="B136" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C136" s="49" t="inlineStr">
@@ -5999,7 +5999,7 @@
       </c>
       <c r="B137" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C137" s="49" t="inlineStr">
@@ -6031,7 +6031,7 @@
       </c>
       <c r="B138" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C138" s="49" t="inlineStr">
@@ -6063,7 +6063,7 @@
       </c>
       <c r="B139" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C139" s="49" t="inlineStr">
@@ -6095,7 +6095,7 @@
       </c>
       <c r="B140" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C140" s="49" t="inlineStr">
@@ -6127,7 +6127,7 @@
       </c>
       <c r="B141" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C141" s="49" t="inlineStr">
@@ -6159,7 +6159,7 @@
       </c>
       <c r="B142" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C142" s="49" t="inlineStr">
@@ -6191,7 +6191,7 @@
       </c>
       <c r="B143" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C143" s="49" t="inlineStr">
@@ -6223,7 +6223,7 @@
       </c>
       <c r="B144" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C144" s="49" t="inlineStr">
@@ -6255,7 +6255,7 @@
       </c>
       <c r="B145" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту. Села А-З.</t>
+          <t>Metric books of Orthodox churches of Zaslavsky district. The villages A-C.</t>
         </is>
       </c>
       <c r="C145" s="49" t="inlineStr">
@@ -6287,7 +6287,7 @@
       </c>
       <c r="B146" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C146" s="49" t="inlineStr">
@@ -6319,7 +6319,7 @@
       </c>
       <c r="B147" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C147" s="49" t="inlineStr">
@@ -6351,7 +6351,7 @@
       </c>
       <c r="B148" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C148" s="49" t="inlineStr">
@@ -6383,7 +6383,7 @@
       </c>
       <c r="B149" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C149" s="49" t="inlineStr">
@@ -6415,7 +6415,7 @@
       </c>
       <c r="B150" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту. Села А-З.</t>
+          <t>Metric books of Orthodox churches of Zaslavsky district. The villages A-C.</t>
         </is>
       </c>
       <c r="C150" s="49" t="inlineStr">
@@ -6447,7 +6447,7 @@
       </c>
       <c r="B151" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C151" s="49" t="inlineStr">
@@ -6479,7 +6479,7 @@
       </c>
       <c r="B152" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C152" s="49" t="inlineStr">
@@ -6511,7 +6511,7 @@
       </c>
       <c r="B153" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C153" s="49" t="inlineStr">
@@ -6543,7 +6543,7 @@
       </c>
       <c r="B154" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Заславського повіту. Села А-Л.</t>
+          <t>Metric books of Orthodox churches of Zaslavsky district. Village A-L.</t>
         </is>
       </c>
       <c r="C154" s="49" t="inlineStr">
@@ -6575,7 +6575,7 @@
       </c>
       <c r="B155" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C155" s="49" t="inlineStr">
@@ -6607,7 +6607,7 @@
       </c>
       <c r="B156" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C156" s="49" t="inlineStr">
@@ -6639,7 +6639,7 @@
       </c>
       <c r="B157" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C157" s="49" t="inlineStr">
@@ -6671,7 +6671,7 @@
       </c>
       <c r="B158" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C158" s="49" t="inlineStr">
@@ -6703,7 +6703,7 @@
       </c>
       <c r="B159" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C159" s="49" t="inlineStr">
@@ -6735,7 +6735,7 @@
       </c>
       <c r="B160" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C160" s="49" t="inlineStr">
@@ -6767,7 +6767,7 @@
       </c>
       <c r="B161" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C161" s="49" t="inlineStr">
@@ -6799,7 +6799,7 @@
       </c>
       <c r="B162" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C162" s="49" t="inlineStr">
@@ -6831,7 +6831,7 @@
       </c>
       <c r="B163" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C163" s="49" t="inlineStr">
@@ -6863,7 +6863,7 @@
       </c>
       <c r="B164" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C164" s="49" t="inlineStr">
@@ -6895,7 +6895,7 @@
       </c>
       <c r="B165" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C165" s="49" t="inlineStr">
@@ -6927,7 +6927,7 @@
       </c>
       <c r="B166" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C166" s="49" t="inlineStr">
@@ -6959,7 +6959,7 @@
       </c>
       <c r="B167" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C167" s="49" t="inlineStr">
@@ -6991,7 +6991,7 @@
       </c>
       <c r="B168" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C168" s="49" t="inlineStr">
@@ -7023,7 +7023,7 @@
       </c>
       <c r="B169" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C169" s="49" t="inlineStr">
@@ -7055,7 +7055,7 @@
       </c>
       <c r="B170" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C170" s="49" t="inlineStr">
@@ -7087,7 +7087,7 @@
       </c>
       <c r="B171" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C171" s="49" t="inlineStr">
@@ -7119,7 +7119,7 @@
       </c>
       <c r="B172" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C172" s="49" t="inlineStr">
@@ -7151,7 +7151,7 @@
       </c>
       <c r="B173" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C173" s="49" t="inlineStr">
@@ -7183,7 +7183,7 @@
       </c>
       <c r="B174" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C174" s="49" t="inlineStr">
@@ -7215,7 +7215,7 @@
       </c>
       <c r="B175" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C175" s="49" t="inlineStr">
@@ -7247,7 +7247,7 @@
       </c>
       <c r="B176" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C176" s="49" t="inlineStr">
@@ -7279,7 +7279,7 @@
       </c>
       <c r="B177" s="48" t="inlineStr">
         <is>
-          <t>Сповідні списки православні А–К</t>
+          <t>Orthodox Lists</t>
         </is>
       </c>
       <c r="C177" s="49" t="inlineStr">
@@ -7311,7 +7311,7 @@
       </c>
       <c r="B178" s="48" t="inlineStr">
         <is>
-          <t>Сповідні розписи православних церков Заславського повіту. Села Р–Я</t>
+          <t>Confessor paintings of the Orthodox churches of Zaslav district. The villages of the r -Y</t>
         </is>
       </c>
       <c r="C178" s="49" t="inlineStr">
@@ -7343,7 +7343,7 @@
       </c>
       <c r="B179" s="48" t="inlineStr">
         <is>
-          <t>Сповідні розписи православних церков Заславського повіту. Села Л–П</t>
+          <t>Confessor paintings of the Orthodox churches of Zaslav district. The villages of L -p</t>
         </is>
       </c>
       <c r="C179" s="49" t="inlineStr">
@@ -7375,7 +7375,7 @@
       </c>
       <c r="B180" s="48" t="inlineStr">
         <is>
-          <t>Сповідні розписи православних церков Заславського повіту. Села Р–Я</t>
+          <t>Confessor paintings of the Orthodox churches of Zaslav district. The villages of the r -Y</t>
         </is>
       </c>
       <c r="C180" s="49" t="inlineStr">
@@ -7407,7 +7407,7 @@
       </c>
       <c r="B181" s="48" t="inlineStr">
         <is>
-          <t>Сповідні розписи православних церков Заславського повіту. Села К–П</t>
+          <t>Confessor paintings of the Orthodox churches of Zaslav district. The villages of K -p</t>
         </is>
       </c>
       <c r="C181" s="49" t="inlineStr">
@@ -7439,7 +7439,7 @@
       </c>
       <c r="B182" s="48" t="inlineStr">
         <is>
-          <t>Сповідні розписи православних церков Заславського повіту. Села А–К</t>
+          <t>Confessor paintings of the Orthodox churches of Zaslav district. Village A -K</t>
         </is>
       </c>
       <c r="C182" s="49" t="inlineStr">
@@ -7471,7 +7471,7 @@
       </c>
       <c r="B183" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга унійної Троїцької церкви с. Дерно (народження 1800-1827), (шлюб 1780-1827) (смерть 1774-1827)</t>
+          <t>Metric book of the Union Trinity Church of the village. Derno (birth 1800-1827), (marriage 1780-1827) (Death 1774-1827)</t>
         </is>
       </c>
       <c r="C183" s="49" t="inlineStr">
@@ -7503,7 +7503,7 @@
       </c>
       <c r="B184" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги унійного Олицького деканату (смерть)</t>
+          <t>Metric books of the union of olive dean (death)</t>
         </is>
       </c>
       <c r="C184" s="49" t="inlineStr">
@@ -7535,7 +7535,7 @@
       </c>
       <c r="B185" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги унійного Олицького деканату (народження)</t>
+          <t>Metric books of the Union Olytsky Deanery (Birth)</t>
         </is>
       </c>
       <c r="C185" s="49" t="inlineStr">
@@ -7567,7 +7567,7 @@
       </c>
       <c r="B186" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги унійного Олицького деканату (смерть)</t>
+          <t>Metric books of the union of olive dean (death)</t>
         </is>
       </c>
       <c r="C186" s="49" t="inlineStr">
@@ -7599,7 +7599,7 @@
       </c>
       <c r="B187" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги унійного Олицького деканату (шлюб)</t>
+          <t>Metric books of the Union Olytsky Deanery (Marriage)</t>
         </is>
       </c>
       <c r="C187" s="49" t="inlineStr">
@@ -7631,7 +7631,7 @@
       </c>
       <c r="B188" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги унійного Олицького деканату (народження)</t>
+          <t>Metric books of the Union Olytsky Deanery (Birth)</t>
         </is>
       </c>
       <c r="C188" s="49" t="inlineStr">
@@ -7663,7 +7663,7 @@
       </c>
       <c r="B189" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги унійного Олицького деканату (народження)</t>
+          <t>Metric books of the Union Olytsky Deanery (Birth)</t>
         </is>
       </c>
       <c r="C189" s="49" t="inlineStr">
@@ -7695,7 +7695,7 @@
       </c>
       <c r="B190" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги унійного Олицького деканату (смерть)</t>
+          <t>Metric books of the union of olive dean (death)</t>
         </is>
       </c>
       <c r="C190" s="49" t="inlineStr">
@@ -7727,7 +7727,7 @@
       </c>
       <c r="B191" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги унійного Олицького деканату. Дубенський повіт. Народження</t>
+          <t>Metric books of the Union Olytsky Deanery. Duben County. Birth</t>
         </is>
       </c>
       <c r="C191" s="49" t="inlineStr">
@@ -7759,7 +7759,7 @@
       </c>
       <c r="B192" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги унійного Олицького деканату. Дубенський повіт. Шлюб</t>
+          <t>Metric books of the Union Olytsky Deanery. Duben County. Marriage</t>
         </is>
       </c>
       <c r="C192" s="49" t="inlineStr">
@@ -7786,12 +7786,12 @@
     <row r="193">
       <c r="A193" s="47" t="inlineStr">
         <is>
-          <t>183а</t>
+          <t>183a</t>
         </is>
       </c>
       <c r="B193" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги (народження)</t>
+          <t>Metric Books (Birth)</t>
         </is>
       </c>
       <c r="C193" s="49" t="inlineStr">
@@ -7823,7 +7823,7 @@
       </c>
       <c r="B194" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги унійного Олицького деканату. Дубенський повіт</t>
+          <t>Metric books of the Union Olytsky Deanery. Duben County</t>
         </is>
       </c>
       <c r="C194" s="49" t="inlineStr">
@@ -7855,7 +7855,7 @@
       </c>
       <c r="B195" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги про народження уніатські (не вся справа)</t>
+          <t>Metric Books on Birth Uniate (not the whole business)</t>
         </is>
       </c>
       <c r="C195" s="49" t="inlineStr">
@@ -7887,7 +7887,7 @@
       </c>
       <c r="B196" s="48" t="inlineStr">
         <is>
-          <t>Сповідні списки православні А–Ж</t>
+          <t>Orthodox Lists Orthodox</t>
         </is>
       </c>
       <c r="C196" s="49" t="inlineStr">
@@ -7919,7 +7919,7 @@
       </c>
       <c r="B197" s="48" t="inlineStr">
         <is>
-          <t>Сповідні розписи православних церков Дубенського повіту. Села З–О</t>
+          <t>Confessor paintings of the Orthodox churches of Dubensky county. The village Z -O</t>
         </is>
       </c>
       <c r="C197" s="49" t="inlineStr">
@@ -7951,7 +7951,7 @@
       </c>
       <c r="B198" s="48" t="inlineStr">
         <is>
-          <t>Сповідні списки православні П–Я</t>
+          <t>Orthodox lists of Orthodox</t>
         </is>
       </c>
       <c r="C198" s="49" t="inlineStr">
@@ -7983,7 +7983,7 @@
       </c>
       <c r="B199" s="48" t="inlineStr">
         <is>
-          <t>Сповідні відомості православних церков Дубенського повіту. Села П-Я.</t>
+          <t>Confessor information of the Orthodox churches of Dubensky county. The villages of P-i.</t>
         </is>
       </c>
       <c r="C199" s="49" t="inlineStr">
@@ -8015,7 +8015,7 @@
       </c>
       <c r="B200" s="48" t="inlineStr">
         <is>
-          <t>Сповідні списки православних церков Дубенського повіту. Села З–О</t>
+          <t>Confessor lists of Orthodox churches of Dubensky county. The village Z -O</t>
         </is>
       </c>
       <c r="C200" s="49" t="inlineStr">
@@ -8047,7 +8047,7 @@
       </c>
       <c r="B201" s="48" t="inlineStr">
         <is>
-          <t>Сповідні списки православні</t>
+          <t>Orthodox lists</t>
         </is>
       </c>
       <c r="C201" s="49" t="inlineStr">
@@ -8079,7 +8079,7 @@
       </c>
       <c r="B202" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга Троїцької церкви с. Милостів Ровенського повіту</t>
+          <t>Metric Book of the Trinity Church of the village The alms of the Rivne county</t>
         </is>
       </c>
       <c r="C202" s="49" t="inlineStr">
@@ -8111,7 +8111,7 @@
       </c>
       <c r="B203" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга греко-уніатських церков Домбровицького благочиння Ровенського повіту. Народження</t>
+          <t>The metric book of the Greek-Uniate Churches of the Dombrovitsky Piety of Rivne County. Birth</t>
         </is>
       </c>
       <c r="C203" s="49" t="inlineStr">
@@ -8143,7 +8143,7 @@
       </c>
       <c r="B204" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга греко-уніатських церков Домбровицького благочиння Ровенського повіту. Шлюб</t>
+          <t>The metric book of the Greek-Uniate Churches of the Dombrovitsky Piety of Rivne County. Marriage</t>
         </is>
       </c>
       <c r="C204" s="49" t="inlineStr">
@@ -8170,12 +8170,12 @@
     <row r="205">
       <c r="A205" s="47" t="inlineStr">
         <is>
-          <t>194а</t>
+          <t>194a</t>
         </is>
       </c>
       <c r="B205" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні (смерть)</t>
+          <t>Orthodox metric books (death)</t>
         </is>
       </c>
       <c r="C205" s="49" t="inlineStr">
@@ -8207,7 +8207,7 @@
       </c>
       <c r="B206" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга греко-уніатських церков Домбровицького благочиння Ровенського повіту. Шлюб</t>
+          <t>The metric book of the Greek-Uniate Churches of the Dombrovitsky Piety of Rivne County. Marriage</t>
         </is>
       </c>
       <c r="C206" s="49" t="inlineStr">
@@ -8239,7 +8239,7 @@
       </c>
       <c r="B207" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга греко-уніатських церков Домбровицького благочиння Ровенського повіту. Народження</t>
+          <t>The metric book of the Greek-Uniate Churches of the Dombrovitsky Piety of Rivne County. Birth</t>
         </is>
       </c>
       <c r="C207" s="49" t="inlineStr">
@@ -8271,7 +8271,7 @@
       </c>
       <c r="B208" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга греко-уніатських церков Домбровицького благочиння Ровенського повіту. Смерть</t>
+          <t>The metric book of the Greek-Uniate Churches of the Dombrovitsky Piety of Rivne County. Death</t>
         </is>
       </c>
       <c r="C208" s="49" t="inlineStr">
@@ -8303,7 +8303,7 @@
       </c>
       <c r="B209" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга церкви Св. Параскеви с. Немовичі Ровенського повіту</t>
+          <t>Metric book of the Church of St. Paraskeva village Nemovichi Rivne County</t>
         </is>
       </c>
       <c r="C209" s="49" t="inlineStr">
@@ -8335,7 +8335,7 @@
       </c>
       <c r="B210" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга греко-уніатських церков Домбровицького благочиння Ровенського повіту. Шлюб</t>
+          <t>The metric book of the Greek-Uniate Churches of the Dombrovitsky Piety of Rivne County. Marriage</t>
         </is>
       </c>
       <c r="C210" s="49" t="inlineStr">
@@ -8367,7 +8367,7 @@
       </c>
       <c r="B211" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга греко-уніатських церков Домбровицького благочиння Ровенського повіту. Смерть</t>
+          <t>The metric book of the Greek-Uniate Churches of the Dombrovitsky Piety of Rivne County. Death</t>
         </is>
       </c>
       <c r="C211" s="49" t="inlineStr">
@@ -8399,7 +8399,7 @@
       </c>
       <c r="B212" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга греко-уніатських церков Домбровицького благочиння Ровенського повіту. Народження</t>
+          <t>The metric book of the Greek-Uniate Churches of the Dombrovitsky Piety of Rivne County. Birth</t>
         </is>
       </c>
       <c r="C212" s="49" t="inlineStr">
@@ -8431,7 +8431,7 @@
       </c>
       <c r="B213" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга греко-уніатських церков Домбровицького благочиння Ровенського повіту. Народження</t>
+          <t>The metric book of the Greek-Uniate Churches of the Dombrovitsky Piety of Rivne County. Birth</t>
         </is>
       </c>
       <c r="C213" s="49" t="inlineStr">
@@ -8463,7 +8463,7 @@
       </c>
       <c r="B214" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга греко-уніатських церков Домбровицького благочиння Ровенського повіту. Смерть</t>
+          <t>The metric book of the Greek-Uniate Churches of the Dombrovitsky Piety of Rivne County. Death</t>
         </is>
       </c>
       <c r="C214" s="49" t="inlineStr">
@@ -8495,7 +8495,7 @@
       </c>
       <c r="B215" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга греко-уніатських церков Домбровицького благочиння Ровенського повіту. Шлюб</t>
+          <t>The metric book of the Greek-Uniate Churches of the Dombrovitsky Piety of Rivne County. Marriage</t>
         </is>
       </c>
       <c r="C215" s="49" t="inlineStr">
@@ -8527,7 +8527,7 @@
       </c>
       <c r="B216" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга греко-уніатських церков Домбровицького благочиння Ровенського повіту. Народження</t>
+          <t>The metric book of the Greek-Uniate Churches of the Dombrovitsky Piety of Rivne County. Birth</t>
         </is>
       </c>
       <c r="C216" s="49" t="inlineStr">
@@ -8559,7 +8559,7 @@
       </c>
       <c r="B217" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга греко-уніатських церков Домбровицького благочиння Ровенського повіту. Смерть</t>
+          <t>The metric book of the Greek-Uniate Churches of the Dombrovitsky Piety of Rivne County. Death</t>
         </is>
       </c>
       <c r="C217" s="49" t="inlineStr">
@@ -8591,7 +8591,7 @@
       </c>
       <c r="B218" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги села Домбровецького. Шлюб</t>
+          <t>Metric books of the village of Dombrovetsky. Marriage</t>
         </is>
       </c>
       <c r="C218" s="49" t="inlineStr">
@@ -8623,7 +8623,7 @@
       </c>
       <c r="B219" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C219" s="49" t="inlineStr">
@@ -8655,7 +8655,7 @@
       </c>
       <c r="B220" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C220" s="49" t="inlineStr">
@@ -8687,7 +8687,7 @@
       </c>
       <c r="B221" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги німців-баптистів</t>
+          <t>Metric books of German Baptists</t>
         </is>
       </c>
       <c r="C221" s="49" t="inlineStr">
@@ -8719,7 +8719,7 @@
       </c>
       <c r="B222" s="48" t="inlineStr">
         <is>
-          <t>Сповідні розписи православних церков Ровенського повіту. Села З–О</t>
+          <t>Confessor paintings of the Orthodox churches of Rivne county. The village Z -O</t>
         </is>
       </c>
       <c r="C222" s="49" t="inlineStr">
@@ -8751,7 +8751,7 @@
       </c>
       <c r="B223" s="48" t="inlineStr">
         <is>
-          <t>Сповідні розписи православних церков Ровенського повіту. Села А–Ж</t>
+          <t>Confessor paintings of the Orthodox churches of Rivne county. Village A -D</t>
         </is>
       </c>
       <c r="C223" s="49" t="inlineStr">
@@ -8783,7 +8783,7 @@
       </c>
       <c r="B224" s="48" t="inlineStr">
         <is>
-          <t>Сповідні відомості православні</t>
+          <t>Orthodox confessions</t>
         </is>
       </c>
       <c r="C224" s="49" t="inlineStr">
@@ -8815,7 +8815,7 @@
       </c>
       <c r="B225" s="48" t="inlineStr">
         <is>
-          <t>Сповідні відомості православних церков Ровенського повіту. Села С–Я</t>
+          <t>Confessor information of the Orthodox churches of Rivne county. The village of C -Y</t>
         </is>
       </c>
       <c r="C225" s="49" t="inlineStr">
@@ -8847,7 +8847,7 @@
       </c>
       <c r="B226" s="48" t="inlineStr">
         <is>
-          <t>Сповідні відомості православних церков Ровенського повіту. Села А–Г</t>
+          <t>Confessor information of the Orthodox churches of Rivne county. Village A -G</t>
         </is>
       </c>
       <c r="C226" s="49" t="inlineStr">
@@ -8879,7 +8879,7 @@
       </c>
       <c r="B227" s="48" t="inlineStr">
         <is>
-          <t>Сповідні розписи православних церков Ровенського повіту. Села Д–К</t>
+          <t>Confessor paintings of the Orthodox churches of Rivne county. The villages of D -K</t>
         </is>
       </c>
       <c r="C227" s="49" t="inlineStr">
@@ -8911,7 +8911,7 @@
       </c>
       <c r="B228" s="48" t="inlineStr">
         <is>
-          <t>Сповідні розписи православних церков Ровенського повіту. Села Л–Р</t>
+          <t>Confessor paintings of the Orthodox churches of Rivne county. The villages of L -r</t>
         </is>
       </c>
       <c r="C228" s="49" t="inlineStr">
@@ -8943,7 +8943,7 @@
       </c>
       <c r="B229" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C229" s="49" t="inlineStr">
@@ -8975,7 +8975,7 @@
       </c>
       <c r="B230" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні (шлюб)</t>
+          <t>Orthodox metric books (marriage)</t>
         </is>
       </c>
       <c r="C230" s="49" t="inlineStr">
@@ -9007,7 +9007,7 @@
       </c>
       <c r="B231" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні (смерть)</t>
+          <t>Orthodox metric books (death)</t>
         </is>
       </c>
       <c r="C231" s="49" t="inlineStr">
@@ -9039,7 +9039,7 @@
       </c>
       <c r="B232" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні (народження)</t>
+          <t>Orthodox Metric Books (Birth)</t>
         </is>
       </c>
       <c r="C232" s="49" t="inlineStr">
@@ -9071,7 +9071,7 @@
       </c>
       <c r="B233" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга греко-католицької Св. Миколаївської церкви с. Вільськ Житомирського повіту. Народження.</t>
+          <t>Metric book of the Greek Catholic St. Nicholas Church Vilsk Zhytomyr County. Birth.</t>
         </is>
       </c>
       <c r="C233" s="49" t="inlineStr">
@@ -9103,7 +9103,7 @@
       </c>
       <c r="B234" s="48" t="inlineStr">
         <is>
-          <t>Метрична книги православні (Кобилин)</t>
+          <t>Orthodox Metric Books (Kobylin)</t>
         </is>
       </c>
       <c r="C234" s="49" t="inlineStr">
@@ -9135,7 +9135,7 @@
       </c>
       <c r="B235" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга с. Ходаки</t>
+          <t>Metric book p. Walks</t>
         </is>
       </c>
       <c r="C235" s="49" t="inlineStr">
@@ -9167,7 +9167,7 @@
       </c>
       <c r="B236" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C236" s="49" t="inlineStr">
@@ -9199,7 +9199,7 @@
       </c>
       <c r="B237" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга м. Ляховці Острозького повіту</t>
+          <t>Metric Book of Lyakhovtsi Ostroh County</t>
         </is>
       </c>
       <c r="C237" s="49" t="inlineStr">
@@ -9231,7 +9231,7 @@
       </c>
       <c r="B238" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні сіл Овруцького повіту</t>
+          <t>Metric books Orthodox villages of Ovruch County</t>
         </is>
       </c>
       <c r="C238" s="49" t="inlineStr">
@@ -9263,7 +9263,7 @@
       </c>
       <c r="B239" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга с. Кобилин</t>
+          <t>Metric book p. Kobylin</t>
         </is>
       </c>
       <c r="C239" s="49" t="inlineStr">
@@ -9295,7 +9295,7 @@
       </c>
       <c r="B240" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C240" s="49" t="inlineStr">
@@ -9327,7 +9327,7 @@
       </c>
       <c r="B241" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C241" s="49" t="inlineStr">
@@ -9359,7 +9359,7 @@
       </c>
       <c r="B242" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга с. Кобилин (народження)</t>
+          <t>Metric book p. Kobilin (Birth)</t>
         </is>
       </c>
       <c r="C242" s="49" t="inlineStr">
@@ -9391,7 +9391,7 @@
       </c>
       <c r="B243" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C243" s="49" t="inlineStr">
@@ -9423,7 +9423,7 @@
       </c>
       <c r="B244" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C244" s="49" t="inlineStr">
@@ -9455,7 +9455,7 @@
       </c>
       <c r="B245" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги села Собичин</t>
+          <t>Metric books of the village Sobychyn</t>
         </is>
       </c>
       <c r="C245" s="49" t="inlineStr">
@@ -9487,7 +9487,7 @@
       </c>
       <c r="B246" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C246" s="49" t="inlineStr">
@@ -9519,7 +9519,7 @@
       </c>
       <c r="B247" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C247" s="49" t="inlineStr">
@@ -9551,7 +9551,7 @@
       </c>
       <c r="B248" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C248" s="49" t="inlineStr">
@@ -9583,7 +9583,7 @@
       </c>
       <c r="B249" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C249" s="49" t="inlineStr">
@@ -9615,7 +9615,7 @@
       </c>
       <c r="B250" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C250" s="49" t="inlineStr">
@@ -9647,7 +9647,7 @@
       </c>
       <c r="B251" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C251" s="49" t="inlineStr">
@@ -9679,7 +9679,7 @@
       </c>
       <c r="B252" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C252" s="49" t="inlineStr">
@@ -9711,7 +9711,7 @@
       </c>
       <c r="B253" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C253" s="49" t="inlineStr">
@@ -9743,7 +9743,7 @@
       </c>
       <c r="B254" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги села Дідковичі</t>
+          <t>Metric books of Didkovichi village</t>
         </is>
       </c>
       <c r="C254" s="49" t="inlineStr">
@@ -9775,7 +9775,7 @@
       </c>
       <c r="B255" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C255" s="49" t="inlineStr">
@@ -9807,7 +9807,7 @@
       </c>
       <c r="B256" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C256" s="49" t="inlineStr">
@@ -9839,7 +9839,7 @@
       </c>
       <c r="B257" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C257" s="49" t="inlineStr">
@@ -9871,7 +9871,7 @@
       </c>
       <c r="B258" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C258" s="49" t="inlineStr">
@@ -9898,12 +9898,12 @@
     <row r="259">
       <c r="A259" s="47" t="inlineStr">
         <is>
-          <t>247а</t>
+          <t>247a</t>
         </is>
       </c>
       <c r="B259" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги села Калинівка (Покровська церква)</t>
+          <t>Metric books of Kalynivka village (Pokrovskaya Church)</t>
         </is>
       </c>
       <c r="C259" s="49" t="inlineStr">
@@ -9935,7 +9935,7 @@
       </c>
       <c r="B260" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C260" s="49" t="inlineStr">
@@ -9967,7 +9967,7 @@
       </c>
       <c r="B261" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C261" s="49" t="inlineStr">
@@ -9999,7 +9999,7 @@
       </c>
       <c r="B262" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга церкви Св. Параскеви с. Кобилівка</t>
+          <t>Metric book of the Church of St. Paraskeva village Kobylivka</t>
         </is>
       </c>
       <c r="C262" s="49" t="inlineStr">
@@ -10031,7 +10031,7 @@
       </c>
       <c r="B263" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C263" s="49" t="inlineStr">
@@ -10063,7 +10063,7 @@
       </c>
       <c r="B264" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C264" s="49" t="inlineStr">
@@ -10095,7 +10095,7 @@
       </c>
       <c r="B265" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C265" s="49" t="inlineStr">
@@ -10127,7 +10127,7 @@
       </c>
       <c r="B266" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C266" s="49" t="inlineStr">
@@ -10159,7 +10159,7 @@
       </c>
       <c r="B267" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C267" s="49" t="inlineStr">
@@ -10191,7 +10191,7 @@
       </c>
       <c r="B268" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C268" s="49" t="inlineStr">
@@ -10223,7 +10223,7 @@
       </c>
       <c r="B269" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C269" s="49" t="inlineStr">
@@ -10255,7 +10255,7 @@
       </c>
       <c r="B270" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C270" s="49" t="inlineStr">
@@ -10287,7 +10287,7 @@
       </c>
       <c r="B271" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C271" s="49" t="inlineStr">
@@ -10319,7 +10319,7 @@
       </c>
       <c r="B272" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C272" s="49" t="inlineStr">
@@ -10351,7 +10351,7 @@
       </c>
       <c r="B273" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C273" s="49" t="inlineStr">
@@ -10383,7 +10383,7 @@
       </c>
       <c r="B274" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга с. Левковичі (народження)</t>
+          <t>Metric book p. Levkovichi (Birth)</t>
         </is>
       </c>
       <c r="C274" s="49" t="inlineStr">
@@ -10415,7 +10415,7 @@
       </c>
       <c r="B275" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга с. Закусили (народження)</t>
+          <t>Metric book p. Snack (birth)</t>
         </is>
       </c>
       <c r="C275" s="49" t="inlineStr">
@@ -10447,7 +10447,7 @@
       </c>
       <c r="B276" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга с. Ходаки (народження)</t>
+          <t>Metric book p. Walkers (birth)</t>
         </is>
       </c>
       <c r="C276" s="49" t="inlineStr">
@@ -10479,7 +10479,7 @@
       </c>
       <c r="B277" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга с. Ходаки (шлюб)</t>
+          <t>Metric book p. Walkers (marriage)</t>
         </is>
       </c>
       <c r="C277" s="49" t="inlineStr">
@@ -10511,7 +10511,7 @@
       </c>
       <c r="B278" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга с. Недашки (народження)</t>
+          <t>Metric book p. Nedes (Birth)</t>
         </is>
       </c>
       <c r="C278" s="49" t="inlineStr">
@@ -10543,7 +10543,7 @@
       </c>
       <c r="B279" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга с. Білошиця</t>
+          <t>Metric book p. Beloshitsa</t>
         </is>
       </c>
       <c r="C279" s="49" t="inlineStr">
@@ -10575,7 +10575,7 @@
       </c>
       <c r="B280" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга с. Дідковичі (народження)</t>
+          <t>Metric book p. Didkovichi (Birth)</t>
         </is>
       </c>
       <c r="C280" s="49" t="inlineStr">
@@ -10607,7 +10607,7 @@
       </c>
       <c r="B281" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга с. Мошки (народження)</t>
+          <t>Metric book p. MOhs (birth)</t>
         </is>
       </c>
       <c r="C281" s="49" t="inlineStr">
@@ -10639,7 +10639,7 @@
       </c>
       <c r="B282" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга с. Михайлівка (народження)</t>
+          <t>Metric book p. Mikhailivka (birth)</t>
         </is>
       </c>
       <c r="C282" s="49" t="inlineStr">
@@ -10671,7 +10671,7 @@
       </c>
       <c r="B283" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C283" s="49" t="inlineStr">
@@ -10703,7 +10703,7 @@
       </c>
       <c r="B284" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C284" s="49" t="inlineStr">
@@ -10735,7 +10735,7 @@
       </c>
       <c r="B285" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга с. Кобилин</t>
+          <t>Metric book p. Kobylin</t>
         </is>
       </c>
       <c r="C285" s="49" t="inlineStr">
@@ -10767,7 +10767,7 @@
       </c>
       <c r="B286" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C286" s="49" t="inlineStr">
@@ -10799,7 +10799,7 @@
       </c>
       <c r="B287" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C287" s="49" t="inlineStr">
@@ -10831,7 +10831,7 @@
       </c>
       <c r="B288" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C288" s="49" t="inlineStr">
@@ -10863,7 +10863,7 @@
       </c>
       <c r="B289" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги Овруцької успенської церкви</t>
+          <t>Metric books of Ovruch Assumption Church</t>
         </is>
       </c>
       <c r="C289" s="49" t="inlineStr">
@@ -10895,7 +10895,7 @@
       </c>
       <c r="B290" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні (Зарічанськ)</t>
+          <t>Orthodox metric books (Zarichansk)</t>
         </is>
       </c>
       <c r="C290" s="49" t="inlineStr">
@@ -10927,7 +10927,7 @@
       </c>
       <c r="B291" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга с. Левковичі (народження)</t>
+          <t>Metric book p. Levkovichi (Birth)</t>
         </is>
       </c>
       <c r="C291" s="49" t="inlineStr">
@@ -10959,7 +10959,7 @@
       </c>
       <c r="B292" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга с. Клочки (народження)</t>
+          <t>Metric book p. Clocks (birth)</t>
         </is>
       </c>
       <c r="C292" s="49" t="inlineStr">
@@ -10991,7 +10991,7 @@
       </c>
       <c r="B293" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга с. Закусили (народження)</t>
+          <t>Metric book p. Snack (birth)</t>
         </is>
       </c>
       <c r="C293" s="49" t="inlineStr">
@@ -11023,7 +11023,7 @@
       </c>
       <c r="B294" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C294" s="49" t="inlineStr">
@@ -11055,7 +11055,7 @@
       </c>
       <c r="B295" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C295" s="49" t="inlineStr">
@@ -11087,7 +11087,7 @@
       </c>
       <c r="B296" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C296" s="49" t="inlineStr">
@@ -11119,7 +11119,7 @@
       </c>
       <c r="B297" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C297" s="49" t="inlineStr">
@@ -11151,7 +11151,7 @@
       </c>
       <c r="B298" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C298" s="49" t="inlineStr">
@@ -11183,7 +11183,7 @@
       </c>
       <c r="B299" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C299" s="49" t="inlineStr">
@@ -11215,7 +11215,7 @@
       </c>
       <c r="B300" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C300" s="49" t="inlineStr">
@@ -11247,7 +11247,7 @@
       </c>
       <c r="B301" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C301" s="49" t="inlineStr">
@@ -11279,7 +11279,7 @@
       </c>
       <c r="B302" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C302" s="49" t="inlineStr">
@@ -11311,7 +11311,7 @@
       </c>
       <c r="B303" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C303" s="49" t="inlineStr">
@@ -11343,7 +11343,7 @@
       </c>
       <c r="B304" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C304" s="49" t="inlineStr">
@@ -11375,7 +11375,7 @@
       </c>
       <c r="B305" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту. Села А–К</t>
+          <t>Metric books of Orthodox churches of Ovruch county. Village A -K</t>
         </is>
       </c>
       <c r="C305" s="49" t="inlineStr">
@@ -11407,7 +11407,7 @@
       </c>
       <c r="B306" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту. Села Л–Ш</t>
+          <t>Metric books of Orthodox churches of Ovruch county. The villages of L -sh</t>
         </is>
       </c>
       <c r="C306" s="49" t="inlineStr">
@@ -11439,7 +11439,7 @@
       </c>
       <c r="B307" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту. Села А–К</t>
+          <t>Metric books of Orthodox churches of Ovruch county. Village A -K</t>
         </is>
       </c>
       <c r="C307" s="49" t="inlineStr">
@@ -11471,7 +11471,7 @@
       </c>
       <c r="B308" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту. Села Л–Ш</t>
+          <t>Metric books of Orthodox churches of Ovruch county. The villages of L -sh</t>
         </is>
       </c>
       <c r="C308" s="49" t="inlineStr">
@@ -11503,7 +11503,7 @@
       </c>
       <c r="B309" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C309" s="49" t="inlineStr">
@@ -11535,7 +11535,7 @@
       </c>
       <c r="B310" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C310" s="49" t="inlineStr">
@@ -11567,7 +11567,7 @@
       </c>
       <c r="B311" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C311" s="49" t="inlineStr">
@@ -11599,7 +11599,7 @@
       </c>
       <c r="B312" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C312" s="49" t="inlineStr">
@@ -11631,7 +11631,7 @@
       </c>
       <c r="B313" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C313" s="49" t="inlineStr">
@@ -11663,7 +11663,7 @@
       </c>
       <c r="B314" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C314" s="49" t="inlineStr">
@@ -11695,7 +11695,7 @@
       </c>
       <c r="B315" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C315" s="49" t="inlineStr">
@@ -11727,7 +11727,7 @@
       </c>
       <c r="B316" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C316" s="49" t="inlineStr">
@@ -11759,7 +11759,7 @@
       </c>
       <c r="B317" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту. Села Л–Щ</t>
+          <t>Metric books of Orthodox churches of Ovruch county. The villages of L -Sh</t>
         </is>
       </c>
       <c r="C317" s="49" t="inlineStr">
@@ -11791,7 +11791,7 @@
       </c>
       <c r="B318" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C318" s="49" t="inlineStr">
@@ -11823,7 +11823,7 @@
       </c>
       <c r="B319" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C319" s="49" t="inlineStr">
@@ -11855,7 +11855,7 @@
       </c>
       <c r="B320" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C320" s="49" t="inlineStr">
@@ -11887,7 +11887,7 @@
       </c>
       <c r="B321" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Житомирського повіту. Житомир, села З-К</t>
+          <t>Metric books of Orthodox churches of Zhytomyr county. Zhytomyr, villages with</t>
         </is>
       </c>
       <c r="C321" s="49" t="inlineStr">
@@ -11919,7 +11919,7 @@
       </c>
       <c r="B322" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C322" s="49" t="inlineStr">
@@ -11951,7 +11951,7 @@
       </c>
       <c r="B323" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C323" s="49" t="inlineStr">
@@ -11983,7 +11983,7 @@
       </c>
       <c r="B324" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C324" s="49" t="inlineStr">
@@ -12015,7 +12015,7 @@
       </c>
       <c r="B325" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C325" s="49" t="inlineStr">
@@ -12047,7 +12047,7 @@
       </c>
       <c r="B326" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C326" s="49" t="inlineStr">
@@ -12079,7 +12079,7 @@
       </c>
       <c r="B327" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C327" s="49" t="inlineStr">
@@ -12111,7 +12111,7 @@
       </c>
       <c r="B328" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C328" s="49" t="inlineStr">
@@ -12143,7 +12143,7 @@
       </c>
       <c r="B329" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C329" s="49" t="inlineStr">
@@ -12175,7 +12175,7 @@
       </c>
       <c r="B330" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту. Села М–Ш</t>
+          <t>Metric books of Orthodox churches of Ovruch county. The villages of M -Sh</t>
         </is>
       </c>
       <c r="C330" s="49" t="inlineStr">
@@ -12207,7 +12207,7 @@
       </c>
       <c r="B331" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C331" s="49" t="inlineStr">
@@ -12239,7 +12239,7 @@
       </c>
       <c r="B332" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C332" s="49" t="inlineStr">
@@ -12271,7 +12271,7 @@
       </c>
       <c r="B333" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C333" s="49" t="inlineStr">
@@ -12303,7 +12303,7 @@
       </c>
       <c r="B334" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C334" s="49" t="inlineStr">
@@ -12335,7 +12335,7 @@
       </c>
       <c r="B335" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга Заручайської Успенської церкви (народження)</t>
+          <t>Metric Book of the Zaruchaysk Assumption Church (Birth)</t>
         </is>
       </c>
       <c r="C335" s="49" t="inlineStr">
@@ -12367,7 +12367,7 @@
       </c>
       <c r="B336" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C336" s="49" t="inlineStr">
@@ -12399,7 +12399,7 @@
       </c>
       <c r="B337" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C337" s="49" t="inlineStr">
@@ -12431,7 +12431,7 @@
       </c>
       <c r="B338" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C338" s="49" t="inlineStr">
@@ -12463,7 +12463,7 @@
       </c>
       <c r="B339" s="48" t="inlineStr">
         <is>
-          <t>Метрична книга с. Васьковичі (народження)</t>
+          <t>Metric book p. Vaskovichi (birth)</t>
         </is>
       </c>
       <c r="C339" s="49" t="inlineStr">
@@ -12495,7 +12495,7 @@
       </c>
       <c r="B340" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C340" s="49" t="inlineStr">
@@ -12527,7 +12527,7 @@
       </c>
       <c r="B341" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C341" s="49" t="inlineStr">
@@ -12559,7 +12559,7 @@
       </c>
       <c r="B342" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C342" s="49" t="inlineStr">
@@ -12591,7 +12591,7 @@
       </c>
       <c r="B343" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C343" s="49" t="inlineStr">
@@ -12623,7 +12623,7 @@
       </c>
       <c r="B344" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C344" s="49" t="inlineStr">
@@ -12655,7 +12655,7 @@
       </c>
       <c r="B345" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C345" s="49" t="inlineStr">
@@ -12687,7 +12687,7 @@
       </c>
       <c r="B346" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C346" s="49" t="inlineStr">
@@ -12719,7 +12719,7 @@
       </c>
       <c r="B347" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C347" s="49" t="inlineStr">
@@ -12751,7 +12751,7 @@
       </c>
       <c r="B348" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C348" s="49" t="inlineStr">
@@ -12783,7 +12783,7 @@
       </c>
       <c r="B349" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C349" s="49" t="inlineStr">
@@ -12815,7 +12815,7 @@
       </c>
       <c r="B350" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C350" s="49" t="inlineStr">
@@ -12847,7 +12847,7 @@
       </c>
       <c r="B351" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C351" s="49" t="inlineStr">
@@ -12879,7 +12879,7 @@
       </c>
       <c r="B352" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту. Села Л–Т</t>
+          <t>Metric books of Orthodox churches of Ovruch county. The villages of L -T</t>
         </is>
       </c>
       <c r="C352" s="49" t="inlineStr">
@@ -12911,7 +12911,7 @@
       </c>
       <c r="B353" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C353" s="49" t="inlineStr">
@@ -12943,7 +12943,7 @@
       </c>
       <c r="B354" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C354" s="49" t="inlineStr">
@@ -12975,7 +12975,7 @@
       </c>
       <c r="B355" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту</t>
+          <t>Metric Books of Orthodox Churches of Ovruch County</t>
         </is>
       </c>
       <c r="C355" s="49" t="inlineStr">
@@ -13007,7 +13007,7 @@
       </c>
       <c r="B356" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту. Села Б-Д.</t>
+          <t>Metric books of Orthodox churches of Ovruch county. The villages of BD.</t>
         </is>
       </c>
       <c r="C356" s="49" t="inlineStr">
@@ -13039,7 +13039,7 @@
       </c>
       <c r="B357" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту. Села Л-Ш</t>
+          <t>Metric books of Orthodox churches of Ovruch county. The villages of L-sh</t>
         </is>
       </c>
       <c r="C357" s="49" t="inlineStr">
@@ -13071,7 +13071,7 @@
       </c>
       <c r="B358" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Овруцького повіту. Села М-Ш</t>
+          <t>Metric books of Orthodox churches of Ovruch county. The villages of M-Sh</t>
         </is>
       </c>
       <c r="C358" s="49" t="inlineStr">
@@ -13103,7 +13103,7 @@
       </c>
       <c r="B359" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Острозького повіту</t>
+          <t>Metric books of Orthodox churches of Ostroh county</t>
         </is>
       </c>
       <c r="C359" s="49" t="inlineStr">
@@ -13135,7 +13135,7 @@
       </c>
       <c r="B360" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Острозького повіту. Див. #Примітки.</t>
+          <t>Metric books of Orthodox churches of Ostroh district. See #Notes.</t>
         </is>
       </c>
       <c r="C360" s="49" t="inlineStr">
@@ -13167,7 +13167,7 @@
       </c>
       <c r="B361" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православних церков Острозького повіту. Див. #Примітки.</t>
+          <t>Metric books of Orthodox churches of Ostroh district. See #Notes.</t>
         </is>
       </c>
       <c r="C361" s="49" t="inlineStr">
@@ -13199,7 +13199,7 @@
       </c>
       <c r="B362" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні відомості села К–Н</t>
+          <t>Confessional information of the village K -H</t>
         </is>
       </c>
       <c r="C362" s="49" t="inlineStr">
@@ -13231,7 +13231,7 @@
       </c>
       <c r="B363" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні відомості православних церков Луцького повіту. Села Р–Я</t>
+          <t>Confessional information of the Orthodox churches of Lutsk county. The villages of the r -Y</t>
         </is>
       </c>
       <c r="C363" s="49" t="inlineStr">
@@ -13263,7 +13263,7 @@
       </c>
       <c r="B364" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні відомості православних церков Овруцького повіту. Села Б–І</t>
+          <t>Confessional information of the Orthodox Churches of Ovruch County. The villages of b - i</t>
         </is>
       </c>
       <c r="C364" s="49" t="inlineStr">
@@ -13295,7 +13295,7 @@
       </c>
       <c r="B365" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні відомості села О–Ш</t>
+          <t>O -W village confessional information</t>
         </is>
       </c>
       <c r="C365" s="49" t="inlineStr">
@@ -13327,7 +13327,7 @@
       </c>
       <c r="B366" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні відомості села П–Ш</t>
+          <t>Confessional information of the village of P -W</t>
         </is>
       </c>
       <c r="C366" s="49" t="inlineStr">
@@ -13359,7 +13359,7 @@
       </c>
       <c r="B367" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні відомості села Г–К</t>
+          <t>Confessional Information of the village of G -K</t>
         </is>
       </c>
       <c r="C367" s="49" t="inlineStr">
@@ -13391,7 +13391,7 @@
       </c>
       <c r="B368" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні відомості села Б–В</t>
+          <t>Confessional Information of the village of B -B</t>
         </is>
       </c>
       <c r="C368" s="49" t="inlineStr">
@@ -13423,7 +13423,7 @@
       </c>
       <c r="B369" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні відомості православних церков Овруцького повіту. Села Л-О.</t>
+          <t>Confessional information of the Orthodox Churches of Ovruch County. The villages of L-o.</t>
         </is>
       </c>
       <c r="C369" s="49" t="inlineStr">
@@ -13455,7 +13455,7 @@
       </c>
       <c r="B370" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C370" s="49" t="inlineStr">
@@ -13487,7 +13487,7 @@
       </c>
       <c r="B371" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C371" s="49" t="inlineStr">
@@ -13519,7 +13519,7 @@
       </c>
       <c r="B372" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C372" s="49" t="inlineStr">
@@ -13551,7 +13551,7 @@
       </c>
       <c r="B373" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C373" s="49" t="inlineStr">
@@ -13583,7 +13583,7 @@
       </c>
       <c r="B374" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C374" s="49" t="inlineStr">
@@ -13615,7 +13615,7 @@
       </c>
       <c r="B375" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C375" s="49" t="inlineStr">
@@ -13647,7 +13647,7 @@
       </c>
       <c r="B376" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C376" s="49" t="inlineStr">
@@ -13679,7 +13679,7 @@
       </c>
       <c r="B377" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C377" s="49" t="inlineStr">
@@ -13711,7 +13711,7 @@
       </c>
       <c r="B378" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C378" s="49" t="inlineStr">
@@ -13743,7 +13743,7 @@
       </c>
       <c r="B379" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C379" s="49" t="inlineStr">
@@ -13775,7 +13775,7 @@
       </c>
       <c r="B380" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C380" s="49" t="inlineStr">
@@ -13807,7 +13807,7 @@
       </c>
       <c r="B381" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C381" s="49" t="inlineStr">
@@ -13839,7 +13839,7 @@
       </c>
       <c r="B382" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C382" s="49" t="inlineStr">
@@ -13871,7 +13871,7 @@
       </c>
       <c r="B383" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C383" s="49" t="inlineStr">
@@ -13903,7 +13903,7 @@
       </c>
       <c r="B384" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C384" s="49" t="inlineStr">
@@ -13935,7 +13935,7 @@
       </c>
       <c r="B385" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C385" s="49" t="inlineStr">
@@ -13967,7 +13967,7 @@
       </c>
       <c r="B386" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C386" s="49" t="inlineStr">
@@ -13999,7 +13999,7 @@
       </c>
       <c r="B387" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C387" s="49" t="inlineStr">
@@ -14031,7 +14031,7 @@
       </c>
       <c r="B388" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C388" s="49" t="inlineStr">
@@ -14063,7 +14063,7 @@
       </c>
       <c r="B389" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C389" s="49" t="inlineStr">
@@ -14095,7 +14095,7 @@
       </c>
       <c r="B390" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C390" s="49" t="inlineStr">
@@ -14127,7 +14127,7 @@
       </c>
       <c r="B391" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C391" s="49" t="inlineStr">
@@ -14159,7 +14159,7 @@
       </c>
       <c r="B392" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C392" s="49" t="inlineStr">
@@ -14191,7 +14191,7 @@
       </c>
       <c r="B393" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C393" s="49" t="inlineStr">
@@ -14223,7 +14223,7 @@
       </c>
       <c r="B394" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C394" s="49" t="inlineStr">
@@ -14255,7 +14255,7 @@
       </c>
       <c r="B395" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C395" s="49" t="inlineStr">
@@ -14287,7 +14287,7 @@
       </c>
       <c r="B396" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C396" s="49" t="inlineStr">
@@ -14319,7 +14319,7 @@
       </c>
       <c r="B397" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C397" s="49" t="inlineStr">
@@ -14351,7 +14351,7 @@
       </c>
       <c r="B398" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C398" s="49" t="inlineStr">
@@ -14383,7 +14383,7 @@
       </c>
       <c r="B399" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C399" s="49" t="inlineStr">
@@ -14415,7 +14415,7 @@
       </c>
       <c r="B400" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C400" s="49" t="inlineStr">
@@ -14447,7 +14447,7 @@
       </c>
       <c r="B401" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C401" s="49" t="inlineStr">
@@ -14479,7 +14479,7 @@
       </c>
       <c r="B402" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C402" s="49" t="inlineStr">
@@ -14511,7 +14511,7 @@
       </c>
       <c r="B403" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C403" s="49" t="inlineStr">
@@ -14543,7 +14543,7 @@
       </c>
       <c r="B404" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C404" s="49" t="inlineStr">
@@ -14575,7 +14575,7 @@
       </c>
       <c r="B405" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C405" s="49" t="inlineStr">
@@ -14607,7 +14607,7 @@
       </c>
       <c r="B406" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C406" s="49" t="inlineStr">
@@ -14639,7 +14639,7 @@
       </c>
       <c r="B407" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C407" s="49" t="inlineStr">
@@ -14671,7 +14671,7 @@
       </c>
       <c r="B408" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні. Див. #Примітки.</t>
+          <t>Metric books are Orthodox. See #Notes.</t>
         </is>
       </c>
       <c r="C408" s="49" t="inlineStr">
@@ -14703,7 +14703,7 @@
       </c>
       <c r="B409" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні відомості</t>
+          <t>Confessional information</t>
         </is>
       </c>
       <c r="C409" s="49" t="inlineStr">
@@ -14735,7 +14735,7 @@
       </c>
       <c r="B410" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні відомості</t>
+          <t>Confessional information</t>
         </is>
       </c>
       <c r="C410" s="49" t="inlineStr">
@@ -14767,7 +14767,7 @@
       </c>
       <c r="B411" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні відомості</t>
+          <t>Confessional information</t>
         </is>
       </c>
       <c r="C411" s="49" t="inlineStr">
@@ -14799,7 +14799,7 @@
       </c>
       <c r="B412" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні відомості</t>
+          <t>Confessional information</t>
         </is>
       </c>
       <c r="C412" s="49" t="inlineStr">
@@ -14831,7 +14831,7 @@
       </c>
       <c r="B413" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C413" s="49" t="inlineStr">
@@ -14863,7 +14863,7 @@
       </c>
       <c r="B414" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C414" s="49" t="inlineStr">
@@ -14895,7 +14895,7 @@
       </c>
       <c r="B415" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C415" s="49" t="inlineStr">
@@ -14927,7 +14927,7 @@
       </c>
       <c r="B416" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C416" s="49" t="inlineStr">
@@ -14959,7 +14959,7 @@
       </c>
       <c r="B417" s="48" t="inlineStr">
         <is>
-          <t>Метричні книги православні</t>
+          <t>Metric books are Orthodox</t>
         </is>
       </c>
       <c r="C417" s="49" t="inlineStr">
@@ -14991,7 +14991,7 @@
       </c>
       <c r="B418" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні відомості православних церков Володимир-Волинського повіту. Села О-Я</t>
+          <t>Confessional information of the Orthodox churches of Vladimir-Volyn district. The village of O-I</t>
         </is>
       </c>
       <c r="C418" s="49" t="inlineStr">
@@ -15023,7 +15023,7 @@
       </c>
       <c r="B419" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні відомості православних церков Володимир-Волинського повіту. Села З-О</t>
+          <t>Confessional information of the Orthodox churches of Vladimir-Volyn district. The village with</t>
         </is>
       </c>
       <c r="C419" s="49" t="inlineStr">
@@ -15055,7 +15055,7 @@
       </c>
       <c r="B420" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні відомості православних церков Володимир-Волинського повіту. Села А-З.</t>
+          <t>Confessional information of the Orthodox churches of Vladimir-Volyn district. The villages A-C.</t>
         </is>
       </c>
       <c r="C420" s="49" t="inlineStr">
@@ -15087,7 +15087,7 @@
       </c>
       <c r="B421" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні відомості православних церков Володимир-Волинського повіту. Села Д-К</t>
+          <t>Confessional information of the Orthodox churches of Vladimir-Volyn district. The villages of D-K</t>
         </is>
       </c>
       <c r="C421" s="49" t="inlineStr">
@@ -15119,7 +15119,7 @@
       </c>
       <c r="B422" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні відомості православних церков Володимир-Волинського повіту. Села А-Д</t>
+          <t>Confessional information of the Orthodox churches of Vladimir-Volyn district. The villages AD</t>
         </is>
       </c>
       <c r="C422" s="49" t="inlineStr">
@@ -15151,7 +15151,7 @@
       </c>
       <c r="B423" s="48" t="inlineStr">
         <is>
-          <t>Сповідальні відомості православних церков Володимир-Волинського повіту. Села Л-О</t>
+          <t>Confessional information of the Orthodox churches of Vladimir-Volyn district. The villages of L-o</t>
         </is>
       </c>
       <c r="C423" s="49" t="inlineStr">

</xml_diff>